<commit_message>
fixed failed tests due to eol differences
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_repeatUntil_assert.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_repeatUntil_assert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8317A69D-289E-435B-8210-1CD54ACF62B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B4BA8-DBC5-4065-85E9-54B3845B9AD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1787,9 +1787,6 @@
     <t>endIndex</t>
   </si>
   <si>
-    <t>-1</t>
-  </si>
-  <si>
     <t>Test RepeatUntil-Assert</t>
   </si>
   <si>
@@ -1842,6 +1839,9 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>120000</t>
   </si>
 </sst>
 </file>
@@ -4548,7 +4548,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4683,10 +4683,10 @@
     </row>
     <row r="5" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
+        <v>570</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>571</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>572</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>13</v>
@@ -4695,7 +4695,7 @@
         <v>69</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -4718,7 +4718,7 @@
         <v>194</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4734,7 +4734,7 @@
     <row r="7" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>13</v>
@@ -4771,7 +4771,7 @@
         <v>569</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -4786,7 +4786,7 @@
     <row r="9" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="37" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>13</v>
@@ -4795,10 +4795,10 @@
         <v>317</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>570</v>
+        <v>588</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -4813,7 +4813,7 @@
     <row r="10" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="B10" s="38" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>51</v>
@@ -4822,10 +4822,10 @@
         <v>29</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>577</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>578</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -4847,7 +4847,7 @@
         <v>69</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -4870,7 +4870,7 @@
         <v>194</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -4896,7 +4896,7 @@
         <v>567</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -4911,7 +4911,7 @@
     <row r="14" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>51</v>
@@ -4920,10 +4920,10 @@
         <v>423</v>
       </c>
       <c r="E14" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>577</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>578</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -4938,7 +4938,7 @@
     <row r="15" spans="1:15" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>13</v>
@@ -4947,7 +4947,7 @@
         <v>377</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -4970,7 +4970,7 @@
         <v>69</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>

</xml_diff>